<commit_message>
tagged message reply task completed
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15885" windowHeight="7815"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -2308,8 +2308,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -2328,7 +2328,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2342,46 +2370,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2395,6 +2386,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -2402,8 +2401,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2418,33 +2432,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2456,8 +2455,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2480,7 +2480,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2498,7 +2510,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2510,7 +2540,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2522,7 +2558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2534,7 +2570,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2552,13 +2588,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2570,13 +2600,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2588,37 +2618,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2630,7 +2642,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2642,25 +2654,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2671,6 +2671,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2685,24 +2694,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2726,17 +2717,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2757,6 +2737,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2771,13 +2760,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2786,136 +2786,136 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3270,8 +3270,8 @@
   <sheetPr/>
   <dimension ref="A1:C382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.82857142857143" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -6401,7 +6401,7 @@
         <v>567</v>
       </c>
       <c r="C284" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285" spans="1:3">

</xml_diff>